<commit_message>
Se implementa copia de rangos con formato y celda destino
</commit_message>
<xml_diff>
--- a/Interop_Python/demo_salida.xlsx
+++ b/Interop_Python/demo_salida.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520AC5A9-4064-4DA7-B25F-F7C82D3E6010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAB6634-4451-4972-B357-7A04E110BA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>Nombre</t>
   </si>
@@ -34,6 +35,21 @@
   </si>
   <si>
     <t>30</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -89,7 +105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -97,6 +113,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,7 +391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -467,4 +484,138 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B4D3E5-DF54-4AE9-B830-D2B9D6983F63}">
+  <dimension ref="C5:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+      <c r="G7" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3">
+        <v>6</v>
+      </c>
+      <c r="G8" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="3">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3">
+        <v>7</v>
+      </c>
+      <c r="G9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="3">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3">
+        <v>7</v>
+      </c>
+      <c r="F10" s="3">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="3">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3">
+        <v>8</v>
+      </c>
+      <c r="F11" s="3">
+        <v>9</v>
+      </c>
+      <c r="G11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mejoras en la copia de datos
</commit_message>
<xml_diff>
--- a/Interop_Python/demo_salida.xlsx
+++ b/Interop_Python/demo_salida.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAB6634-4451-4972-B357-7A04E110BA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759EE2FF-548A-4632-B142-E69B4E2279CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,20 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -488,15 +501,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B4D3E5-DF54-4AE9-B830-D2B9D6983F63}">
-  <dimension ref="C5:G11"/>
+  <dimension ref="C5:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -513,7 +526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="3">
         <v>1</v>
       </c>
@@ -530,7 +543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -547,7 +560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="3">
         <v>3</v>
       </c>
@@ -564,7 +577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="3">
         <v>4</v>
       </c>
@@ -581,7 +594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" s="3">
         <v>5</v>
       </c>
@@ -597,8 +610,12 @@
       <c r="G10" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f>SUM(C6:G11)</f>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" s="3">
         <v>6</v>
       </c>

</xml_diff>